<commit_message>
Charts oil, natural gas e LNG
</commit_message>
<xml_diff>
--- a/SUT/Aggregations/IOT_agg.xlsx
+++ b/SUT/Aggregations/IOT_agg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\IEA10Steps\Aggregations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\IEA10Steps\SUT\Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BACCBAC-F0C0-42FE-990D-FD3D61AA04E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23E93FC-8801-4039-8EB5-AA6EF551A2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="1344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="1349">
   <si>
     <t>Aggregation</t>
   </si>
@@ -4068,6 +4068,21 @@
   </si>
   <si>
     <t>High-skilled Employment</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Latin America</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Middle East</t>
   </si>
 </sst>
 </file>
@@ -13517,8 +13532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13757,7 +13772,7 @@
         <v>1149</v>
       </c>
       <c r="B30" t="s">
-        <v>1336</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -13861,7 +13876,7 @@
         <v>1162</v>
       </c>
       <c r="B43" t="s">
-        <v>1336</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -13893,7 +13908,7 @@
         <v>1166</v>
       </c>
       <c r="B47" t="s">
-        <v>1336</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -13909,7 +13924,7 @@
         <v>1168</v>
       </c>
       <c r="B49" t="s">
-        <v>1336</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -13917,7 +13932,7 @@
         <v>1169</v>
       </c>
       <c r="B50" t="s">
-        <v>1336</v>
+        <v>1348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>